<commit_message>
remove mentions of changes to line 165
</commit_message>
<xml_diff>
--- a/src/_data/DecemberServiceChanges_ForTranslation_110722.xlsx
+++ b/src/_data/DecemberServiceChanges_ForTranslation_110722.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\kinn\LACMTA\mybus-v2\src\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E0FB15-13CF-4AAD-9B04-DB54A97DD168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F92F016-F4CC-4EC0-8583-81E25A87D5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{74511CEA-1533-4444-8EE6-7F2FEED10AC8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="592">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -11149,267 +11149,6 @@
     <t xml:space="preserve">Маршрут 164: в период повышенного спроса и в обеденное время в будни частота движения автобусов будет увеличена, промежутки между рейсами уменьшатся с 20 до 15 минут. </t>
   </si>
   <si>
-    <t>165 - Improve weekday evening frequency from every 20-60 minutes to every 15-60 minutes.</t>
-  </si>
-  <si>
-    <t>165 – Mejorar la frecuencia de la noche entre semana de cada 20 a 60 minutos a cada 15 a 60 minutos.</t>
-  </si>
-  <si>
-    <r>
-      <t>165 -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="PMingLiU"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 週間晚間的班次時間間隔從每</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>20-60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="PMingLiU"/>
-        <family val="1"/>
-      </rPr>
-      <t>分鐘一班縮短為每</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>15-60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="PMingLiU"/>
-        <family val="1"/>
-      </rPr>
-      <t>分鐘一班。</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>165</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Sylfaen"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">՝ Բարելավել աշխատանքային օրերի երեկոյան հաճախականությունը յուրաքանչյուր </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">20-60 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Sylfaen"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">րոպեի փոխարեն մինչև </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">15-60 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Sylfaen"/>
-        <family val="1"/>
-      </rPr>
-      <t>րոպեն մեկ:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>165</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> - 평일 저녁 시간 운행 간격을 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-        <charset val="129"/>
-      </rPr>
-      <t>~</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">분에서 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-        <charset val="129"/>
-      </rPr>
-      <t>~</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Batang"/>
-        <family val="1"/>
-        <charset val="129"/>
-      </rPr>
-      <t>분으로 개선합니다.</t>
-    </r>
-  </si>
-  <si>
-    <t>165 - Tăng tần suất từ 20-60 phút một chuyến thành 15-60 phút một chuyến vào tối các ngày thường trong tuần.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>165</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="MS Mincho"/>
-        <family val="1"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve"> - 平日夜間の運行本数を</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>20～60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="MS Mincho"/>
-        <family val="1"/>
-        <charset val="128"/>
-      </rPr>
-      <t>分間隔から</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>15～60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="MS Mincho"/>
-        <family val="1"/>
-        <charset val="128"/>
-      </rPr>
-      <t>分間隔に改正。</t>
-    </r>
-  </si>
-  <si>
-    <t>Маршрут 165: в вечернее время будет увеличена частота движения автобусов в будни, промежутки между рейсами уменьшатся с 20–60 до 15–60 минут.</t>
-  </si>
-  <si>
     <t>166 - Improve weekday peak frequency from every 15-20 minutes to every 15 minutes. Improve weekday midday frequency from every 20 minutes to every 15 minutes.</t>
   </si>
   <si>
@@ -23051,12 +22790,12 @@
     <t>206 - Improve weekday midday frequency from every 20 minutes to every 15 minutes. Improve Saturday/Sunday frequency from every 30 minutes to every 20 minutes.</t>
   </si>
   <si>
-    <t>Weekday: 10, 14, 20, 37, 38, 40, 55, 60, 62, 76, 78, 94, 108, 110, 115, 117, 120, 125, 127, 134, 150, 152, 162, 164, 165, 166, 177, 179, 204, 206, 212, 222, 232, 233, 234, 240, 246, 258, 260, 267, 268, 287, 344, 460, 501, 577, 603, 605, 617, 662, 754</t>
+    <t>Weekday: 10, 14, 20, 37, 38, 40, 55, 60, 62, 76, 78, 94, 108, 110, 115, 117, 120, 125, 127, 134, 150, 152, 162, 164, 166, 177, 179, 204, 206, 212, 222, 232, 233, 234, 240, 246, 258, 260, 267, 268, 287, 344, 460, 501, 577, 603, 605, 617, 662, 754</t>
   </si>
   <si>
     <t>Entre semana: 10, 14, 20, 37, 38, 40, 55, 60,
 62, 76, 78, 94, 108, 110, 115, 117, 120, 125,
-127, 134, 150, 152, 162, 164, 165, 166,
+127, 134, 150, 152, 162, 164, 166,
 177, 179, 204, 206, 212, 222, 232, 233, 234,
 240, 246, 258, 260, 267, 268, 287, 344, 460,
 501, 577, 603, 605, 617, 662, 754</t>
@@ -23516,14 +23255,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>164</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="è¨íÀñæí© Pr6N M"/>
-        <family val="2"/>
+      <t>164、166</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="PMingLiU"/>
+        <family val="1"/>
       </rPr>
       <t>、</t>
     </r>
@@ -23535,7 +23274,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>165</t>
+      <t>177</t>
     </r>
     <r>
       <rPr>
@@ -23554,7 +23293,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>166</t>
+      <t>179</t>
     </r>
     <r>
       <rPr>
@@ -23573,7 +23312,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>177</t>
+      <t>182</t>
     </r>
     <r>
       <rPr>
@@ -23592,7 +23331,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>179</t>
+      <t>204</t>
     </r>
     <r>
       <rPr>
@@ -23611,7 +23350,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>182</t>
+      <t>206</t>
     </r>
     <r>
       <rPr>
@@ -23630,7 +23369,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>204</t>
+      <t>212</t>
     </r>
     <r>
       <rPr>
@@ -23649,7 +23388,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>206</t>
+      <t>222</t>
     </r>
     <r>
       <rPr>
@@ -23668,7 +23407,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>212</t>
+      <t>232</t>
     </r>
     <r>
       <rPr>
@@ -23687,7 +23426,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>222</t>
+      <t>233</t>
     </r>
     <r>
       <rPr>
@@ -23706,7 +23445,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>232</t>
+      <t>234</t>
     </r>
     <r>
       <rPr>
@@ -23725,7 +23464,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>233</t>
+      <t>240</t>
     </r>
     <r>
       <rPr>
@@ -23744,7 +23483,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>234</t>
+      <t>246</t>
     </r>
     <r>
       <rPr>
@@ -23763,7 +23502,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>240</t>
+      <t>258</t>
     </r>
     <r>
       <rPr>
@@ -23782,7 +23521,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>246</t>
+      <t>260</t>
     </r>
     <r>
       <rPr>
@@ -23801,7 +23540,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>258</t>
+      <t>267</t>
     </r>
     <r>
       <rPr>
@@ -23820,7 +23559,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>260</t>
+      <t>268</t>
     </r>
     <r>
       <rPr>
@@ -23839,7 +23578,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>267</t>
+      <t>287</t>
     </r>
     <r>
       <rPr>
@@ -23858,7 +23597,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>268</t>
+      <t>344</t>
     </r>
     <r>
       <rPr>
@@ -23877,7 +23616,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>287</t>
+      <t>460</t>
     </r>
     <r>
       <rPr>
@@ -23896,7 +23635,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>344</t>
+      <t>501</t>
     </r>
     <r>
       <rPr>
@@ -23915,7 +23654,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>460</t>
+      <t>577</t>
     </r>
     <r>
       <rPr>
@@ -23934,7 +23673,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>501</t>
+      <t>603</t>
     </r>
     <r>
       <rPr>
@@ -23953,7 +23692,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>577</t>
+      <t>605</t>
     </r>
     <r>
       <rPr>
@@ -23972,7 +23711,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>603</t>
+      <t>617</t>
     </r>
     <r>
       <rPr>
@@ -23991,7 +23730,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>605</t>
+      <t>662</t>
     </r>
     <r>
       <rPr>
@@ -24010,44 +23749,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>617</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="PMingLiU"/>
-        <family val="1"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>662</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="PMingLiU"/>
-        <family val="1"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>754</t>
     </r>
   </si>
@@ -24062,7 +23763,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0, 14, 20, 37, 38, 40, 55, 60, 62, 76, 78, 94, 108, 110, 115, 117, 120, 125, 127, 134, 150, 152, 162, 164, 165, 166, 177, 179, 182, 204, 206, 212, 222, 232, 233, 234, 240, 246, 258, 260, 267, 268, 287, 344, 460, 501, 577, 603, 605, 617, 662, 754</t>
+      <t>0, 14, 20, 37, 38, 40, 55, 60, 62, 76, 78, 94, 108, 110, 115, 117, 120, 125, 127, 134, 150, 152, 162, 164, 166, 177, 179, 182, 204, 206, 212, 222, 232, 233, 234, 240, 246, 258, 260, 267, 268, 287, 344, 460, 501, 577, 603, 605, 617, 662, 754</t>
     </r>
   </si>
   <si>
@@ -24082,11 +23783,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 10, 14, 20, 37, 38, 40, 55, 60, 62, 76, 78, 94, 108, 110, 115, 117, 120, 125, 127, 134, 150, 152, 162, 164, 165, 166, 177, 179, 182, 204, 206, 212, 222, 232, 233, 234, 240, 246, 258, 260, 267, 268, 287, 344, 460, 501, 577, 603, 605, 617, 662, 754</t>
-    </r>
-  </si>
-  <si>
-    <t>Các ngày thường trong tuần: 10, 14, 20, 37, 38, 40, 55, 60, 62, 76, 78, 94, 108, 110, 115, 117, 120, 125, 127, 134, 150, 152, 162, 164, 165, 166, 177, 179, 182, 204, 206, 212, 222, 232, 233, 234, 240, 246, 258, 260, 267, 268, 287, 344, 460, 501, 577, 603, 605, 617, 662, 754</t>
+      <t xml:space="preserve"> 10, 14, 20, 37, 38, 40, 55, 60, 62, 76, 78, 94, 108, 110, 115, 117, 120, 125, 127, 134, 150, 152, 162, 164, 166, 177, 179, 182, 204, 206, 212, 222, 232, 233, 234, 240, 246, 258, 260, 267, 268, 287, 344, 460, 501, 577, 603, 605, 617, 662, 754</t>
+    </r>
+  </si>
+  <si>
+    <t>Các ngày thường trong tuần: 10, 14, 20, 37, 38, 40, 55, 60, 62, 76, 78, 94, 108, 110, 115, 117, 120, 125, 127, 134, 150, 152, 162, 164, 166, 177, 179, 182, 204, 206, 212, 222, 232, 233, 234, 240, 246, 258, 260, 267, 268, 287, 344, 460, 501, 577, 603, 605, 617, 662, 754</t>
   </si>
   <si>
     <r>
@@ -24098,11 +23799,11 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>10, 14, 20, 37, 38, 40, 55, 60, 62, 76, 78, 94, 108, 110, 115, 117, 120, 125, 127, 134, 150, 152, 162, 164, 165, 166, 177, 179, 182, 204, 206, 212, 222, 232, 233, 234, 240, 246, 258, 260, 267, 268, 287, 344, 460, 501, 577, 603, 605, 617, 662, 754</t>
-    </r>
-  </si>
-  <si>
-    <t>В будни: 10, 14, 20, 37, 38, 40, 55, 60, 62, 76, 78, 94, 108, 110, 115, 117, 120, 125, 127, 134, 150, 152, 162, 164, 165, 166, 177, 179, 182, 204, 206, 212, 222, 232, 233, 234, 240, 246, 258, 260, 267, 268, 287, 344, 460, 501, 577, 603, 605, 617, 662, 754</t>
+      <t>10, 14, 20, 37, 38, 40, 55, 60, 62, 76, 78, 94, 108, 110, 115, 117, 120, 125, 127, 134, 150, 152, 162, 164, 166, 177, 179, 182, 204, 206, 212, 222, 232, 233, 234, 240, 246, 258, 260, 267, 268, 287, 344, 460, 501, 577, 603, 605, 617, 662, 754</t>
+    </r>
+  </si>
+  <si>
+    <t>В будни: 10, 14, 20, 37, 38, 40, 55, 60, 62, 76, 78, 94, 108, 110, 115, 117, 120, 125, 127, 134, 150, 152, 162, 164, 166, 177, 179, 182, 204, 206, 212, 222, 232, 233, 234, 240, 246, 258, 260, 267, 268, 287, 344, 460, 501, 577, 603, 605, 617, 662, 754</t>
   </si>
 </sst>
 </file>
@@ -24927,10 +24628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7E4D96-AB3C-6C4D-8226-B104872A4E89}">
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.5" defaultRowHeight="15"/>
@@ -25073,28 +24774,28 @@
     </row>
     <row r="6" spans="1:8" ht="105">
       <c r="A6" s="2" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="H6" s="33" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45">
@@ -25281,7 +24982,7 @@
     </row>
     <row r="14" spans="1:8" ht="86.25" thickBot="1">
       <c r="A14" s="2" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>96</v>
@@ -25307,7 +25008,7 @@
     </row>
     <row r="15" spans="1:8" ht="72" thickBot="1">
       <c r="A15" s="2" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>103</v>
@@ -25333,7 +25034,7 @@
     </row>
     <row r="16" spans="1:8" ht="135.75" thickBot="1">
       <c r="A16" s="2" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>110</v>
@@ -25593,7 +25294,7 @@
     </row>
     <row r="26" spans="1:8" ht="60.75" thickBot="1">
       <c r="A26" s="2" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>189</v>
@@ -25775,7 +25476,7 @@
     </row>
     <row r="33" spans="1:8" ht="100.5" thickBot="1">
       <c r="A33" s="2" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>244</v>
@@ -25929,7 +25630,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="60.75" thickBot="1">
+    <row r="39" spans="1:8" ht="105.75" thickBot="1">
       <c r="A39" s="2" t="s">
         <v>291</v>
       </c>
@@ -25948,14 +25649,14 @@
       <c r="F39" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="G39" s="46" t="s">
+      <c r="G39" s="47" t="s">
         <v>297</v>
       </c>
       <c r="H39" s="38" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="105.75" thickBot="1">
+    <row r="40" spans="1:8" ht="72" thickBot="1">
       <c r="A40" s="2" t="s">
         <v>299</v>
       </c>
@@ -25974,7 +25675,7 @@
       <c r="F40" s="38" t="s">
         <v>304</v>
       </c>
-      <c r="G40" s="47" t="s">
+      <c r="G40" s="46" t="s">
         <v>305</v>
       </c>
       <c r="H40" s="38" t="s">
@@ -26007,7 +25708,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="72" thickBot="1">
+    <row r="42" spans="1:8" ht="105.75" thickBot="1">
       <c r="A42" s="2" t="s">
         <v>315</v>
       </c>
@@ -26026,14 +25727,14 @@
       <c r="F42" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="G42" s="46" t="s">
+      <c r="G42" s="47" t="s">
         <v>321</v>
       </c>
       <c r="H42" s="38" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="105.75" thickBot="1">
+    <row r="43" spans="1:8" ht="79.5" thickBot="1">
       <c r="A43" s="2" t="s">
         <v>323</v>
       </c>
@@ -26052,14 +25753,14 @@
       <c r="F43" s="38" t="s">
         <v>328</v>
       </c>
-      <c r="G43" s="47" t="s">
+      <c r="G43" s="46" t="s">
         <v>329</v>
       </c>
       <c r="H43" s="38" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="79.5" thickBot="1">
+    <row r="44" spans="1:8" ht="60.75" thickBot="1">
       <c r="A44" s="2" t="s">
         <v>331</v>
       </c>
@@ -26085,7 +25786,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="60.75" thickBot="1">
+    <row r="45" spans="1:8" ht="112.5" thickBot="1">
       <c r="A45" s="2" t="s">
         <v>339</v>
       </c>
@@ -26111,35 +25812,35 @@
         <v>346</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="112.5" thickBot="1">
+    <row r="46" spans="1:8" ht="100.5" thickBot="1">
       <c r="A46" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="D46" s="24" t="s">
         <v>349</v>
       </c>
-      <c r="D46" s="24" t="s">
+      <c r="E46" s="32" t="s">
         <v>350</v>
       </c>
-      <c r="E46" s="32" t="s">
+      <c r="F46" s="38" t="s">
         <v>351</v>
       </c>
-      <c r="F46" s="38" t="s">
+      <c r="G46" s="46" t="s">
         <v>352</v>
       </c>
-      <c r="G46" s="46" t="s">
+      <c r="H46" s="38" t="s">
         <v>353</v>
       </c>
-      <c r="H46" s="38" t="s">
+    </row>
+    <row r="47" spans="1:8" ht="150.75" thickBot="1">
+      <c r="A47" s="2" t="s">
         <v>354</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="100.5" thickBot="1">
-      <c r="A47" s="2" t="s">
-        <v>591</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>355</v>
@@ -26163,7 +25864,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="150.75" thickBot="1">
+    <row r="48" spans="1:8" ht="48" thickBot="1">
       <c r="A48" s="2" t="s">
         <v>362</v>
       </c>
@@ -26182,18 +25883,18 @@
       <c r="F48" s="38" t="s">
         <v>367</v>
       </c>
-      <c r="G48" s="46" t="s">
+      <c r="G48" s="47" t="s">
         <v>368</v>
       </c>
       <c r="H48" s="38" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="48" thickBot="1">
+    <row r="49" spans="1:8" ht="86.25" thickBot="1">
       <c r="A49" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>371</v>
       </c>
       <c r="C49" s="13" t="s">
@@ -26208,18 +25909,18 @@
       <c r="F49" s="38" t="s">
         <v>375</v>
       </c>
-      <c r="G49" s="47" t="s">
+      <c r="G49" s="46" t="s">
         <v>376</v>
       </c>
       <c r="H49" s="38" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="86.25" thickBot="1">
+    <row r="50" spans="1:8" ht="72" thickBot="1">
       <c r="A50" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>379</v>
       </c>
       <c r="C50" s="13" t="s">
@@ -26234,14 +25935,14 @@
       <c r="F50" s="38" t="s">
         <v>383</v>
       </c>
-      <c r="G50" s="46" t="s">
+      <c r="G50" s="47" t="s">
         <v>384</v>
       </c>
       <c r="H50" s="38" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="72" thickBot="1">
+    <row r="51" spans="1:8" ht="105.75" thickBot="1">
       <c r="A51" s="2" t="s">
         <v>386</v>
       </c>
@@ -26260,7 +25961,7 @@
       <c r="F51" s="38" t="s">
         <v>391</v>
       </c>
-      <c r="G51" s="47" t="s">
+      <c r="G51" s="46" t="s">
         <v>392</v>
       </c>
       <c r="H51" s="38" t="s">
@@ -26286,7 +25987,7 @@
       <c r="F52" s="38" t="s">
         <v>399</v>
       </c>
-      <c r="G52" s="46" t="s">
+      <c r="G52" s="47" t="s">
         <v>400</v>
       </c>
       <c r="H52" s="38" t="s">
@@ -26319,7 +26020,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="105.75" thickBot="1">
+    <row r="54" spans="1:8" ht="72" thickBot="1">
       <c r="A54" s="2" t="s">
         <v>410</v>
       </c>
@@ -26345,11 +26046,11 @@
         <v>417</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="72" thickBot="1">
+    <row r="55" spans="1:8" ht="150.75" thickBot="1">
       <c r="A55" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>419</v>
       </c>
       <c r="C55" s="13" t="s">
@@ -26371,14 +26072,14 @@
         <v>425</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="150.75" thickBot="1">
+    <row r="56" spans="1:8" ht="57.75" thickBot="1">
       <c r="A56" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="15" t="s">
         <v>428</v>
       </c>
       <c r="D56" s="24" t="s">
@@ -26397,14 +26098,14 @@
         <v>433</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="57.75" thickBot="1">
+    <row r="57" spans="1:8" ht="129" thickBot="1">
       <c r="A57" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="13" t="s">
         <v>436</v>
       </c>
       <c r="D57" s="24" t="s">
@@ -26423,11 +26124,11 @@
         <v>441</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="129" thickBot="1">
+    <row r="58" spans="1:8" ht="60.75" thickBot="1">
       <c r="A58" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="2" t="s">
         <v>443</v>
       </c>
       <c r="C58" s="13" t="s">
@@ -26449,7 +26150,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="60.75" thickBot="1">
+    <row r="59" spans="1:8" ht="72" thickBot="1">
       <c r="A59" s="2" t="s">
         <v>450</v>
       </c>
@@ -26527,11 +26228,11 @@
         <v>473</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="72" thickBot="1">
+    <row r="62" spans="1:8" ht="150.75" thickBot="1">
       <c r="A62" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="3" t="s">
         <v>475</v>
       </c>
       <c r="C62" s="13" t="s">
@@ -26546,18 +26247,18 @@
       <c r="F62" s="38" t="s">
         <v>479</v>
       </c>
-      <c r="G62" s="47" t="s">
+      <c r="G62" s="46" t="s">
         <v>480</v>
       </c>
       <c r="H62" s="38" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="150.75" thickBot="1">
+    <row r="63" spans="1:8" ht="72" thickBot="1">
       <c r="A63" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>483</v>
       </c>
       <c r="C63" s="13" t="s">
@@ -26579,7 +26280,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="72" thickBot="1">
+    <row r="64" spans="1:8" ht="105.75" thickBot="1">
       <c r="A64" s="2" t="s">
         <v>490</v>
       </c>
@@ -26605,7 +26306,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="105.75" thickBot="1">
+    <row r="65" spans="1:8" ht="202.5" thickBot="1">
       <c r="A65" s="2" t="s">
         <v>498</v>
       </c>
@@ -26631,7 +26332,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="202.5" thickBot="1">
+    <row r="66" spans="1:8" ht="72" thickBot="1">
       <c r="A66" s="2" t="s">
         <v>506</v>
       </c>
@@ -26683,7 +26384,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="72" thickBot="1">
+    <row r="68" spans="1:8" ht="60.75" thickBot="1">
       <c r="A68" s="2" t="s">
         <v>522</v>
       </c>
@@ -26709,7 +26410,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="60.75" thickBot="1">
+    <row r="69" spans="1:8" ht="90.75" thickBot="1">
       <c r="A69" s="2" t="s">
         <v>530</v>
       </c>
@@ -26735,7 +26436,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="90.75" thickBot="1">
+    <row r="70" spans="1:8" ht="57.75" thickBot="1">
       <c r="A70" s="2" t="s">
         <v>538</v>
       </c>
@@ -26761,7 +26462,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="57.75" thickBot="1">
+    <row r="71" spans="1:8" ht="72" thickBot="1">
       <c r="A71" s="2" t="s">
         <v>546</v>
       </c>
@@ -26787,7 +26488,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="72" thickBot="1">
+    <row r="72" spans="1:8" ht="57.75" thickBot="1">
       <c r="A72" s="2" t="s">
         <v>554</v>
       </c>
@@ -26839,7 +26540,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="57.75" thickBot="1">
+    <row r="74" spans="1:8" ht="72" thickBot="1">
       <c r="A74" s="2" t="s">
         <v>570</v>
       </c>
@@ -26865,34 +26566,8 @@
         <v>577</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="72" thickBot="1">
-      <c r="A75" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="C75" s="13" t="s">
-        <v>580</v>
-      </c>
-      <c r="D75" s="24" t="s">
-        <v>581</v>
-      </c>
-      <c r="E75" s="32" t="s">
-        <v>582</v>
-      </c>
-      <c r="F75" s="38" t="s">
-        <v>583</v>
-      </c>
-      <c r="G75" s="46" t="s">
-        <v>584</v>
-      </c>
-      <c r="H75" s="38" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
-      <c r="B76" s="2"/>
+    <row r="75" spans="1:8">
+      <c r="B75" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>